<commit_message>
Major Change in Learning Rate Schdeduler
</commit_message>
<xml_diff>
--- a/Tool/File_Detail.xlsx
+++ b/Tool/File_Detail.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Li_Duan\Desktop\LSTM-AutoEncoder\Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F8DDD4-0AB4-4956-93AE-339302CD7BFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD27DFCF-1859-43A7-A75D-805316325B9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="162">
   <si>
     <t>Name</t>
   </si>
@@ -408,6 +408,117 @@
   </si>
   <si>
     <t>Remark</t>
+  </si>
+  <si>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>towel</t>
+  </si>
+  <si>
+    <t>shirt</t>
+  </si>
+  <si>
+    <t>sweater</t>
+  </si>
+  <si>
+    <t>tshirt</t>
+  </si>
+  <si>
+    <t>pa1m1</t>
+  </si>
+  <si>
+    <t>pa1m2</t>
+  </si>
+  <si>
+    <t>pa1m3</t>
+  </si>
+  <si>
+    <t>pa1m4</t>
+  </si>
+  <si>
+    <t>pa1m5</t>
+  </si>
+  <si>
+    <t>pa1m6</t>
+  </si>
+  <si>
+    <t>pa1m7</t>
+  </si>
+  <si>
+    <t>pa1m8</t>
+  </si>
+  <si>
+    <t>pa1m9</t>
+  </si>
+  <si>
+    <t>pa1m10</t>
+  </si>
+  <si>
+    <t>pa2m1</t>
+  </si>
+  <si>
+    <t>pa2m2</t>
+  </si>
+  <si>
+    <t>pa2m3</t>
+  </si>
+  <si>
+    <t>pa2m4</t>
+  </si>
+  <si>
+    <t>pa2m5</t>
+  </si>
+  <si>
+    <t>pa2m6</t>
+  </si>
+  <si>
+    <t>pa2m7</t>
+  </si>
+  <si>
+    <t>pa2m8</t>
+  </si>
+  <si>
+    <t>pa2m9</t>
+  </si>
+  <si>
+    <t>pa2m10</t>
+  </si>
+  <si>
+    <t>pa3m1</t>
+  </si>
+  <si>
+    <t>pa3m2</t>
+  </si>
+  <si>
+    <t>pa3m3</t>
+  </si>
+  <si>
+    <t>pa3m4</t>
+  </si>
+  <si>
+    <t>pa3m5</t>
+  </si>
+  <si>
+    <t>pa3m6</t>
+  </si>
+  <si>
+    <t>pa3m7</t>
+  </si>
+  <si>
+    <t>pa3m8</t>
+  </si>
+  <si>
+    <t>pa3m9</t>
+  </si>
+  <si>
+    <t>pa3m10</t>
+  </si>
+  <si>
+    <t>pant</t>
   </si>
 </sst>
 </file>
@@ -731,15 +842,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F120"/>
+  <dimension ref="A1:K150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="B150" sqref="B150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="8" max="8" width="19.54296875" customWidth="1"/>
+    <col min="9" max="9" width="15.7265625" customWidth="1"/>
+    <col min="11" max="11" width="10.6328125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -758,8 +874,17 @@
       <c r="F1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I1" t="s">
+        <v>126</v>
+      </c>
+      <c r="K1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -777,8 +902,17 @@
         <f>D2*3</f>
         <v>315</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H2" t="s">
+        <v>128</v>
+      </c>
+      <c r="I2">
+        <v>10</v>
+      </c>
+      <c r="K2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -796,8 +930,17 @@
         <f t="shared" ref="E3:E66" si="0">D3*3</f>
         <v>900</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H3" t="s">
+        <v>128</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+      <c r="K3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -815,8 +958,17 @@
         <f t="shared" si="0"/>
         <v>939</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H4" t="s">
+        <v>128</v>
+      </c>
+      <c r="I4">
+        <v>10</v>
+      </c>
+      <c r="K4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -834,8 +986,17 @@
         <f t="shared" si="0"/>
         <v>1062</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H5" t="s">
+        <v>129</v>
+      </c>
+      <c r="I5">
+        <v>10</v>
+      </c>
+      <c r="K5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -853,8 +1014,17 @@
         <f t="shared" si="0"/>
         <v>1155</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H6" t="s">
+        <v>129</v>
+      </c>
+      <c r="I6">
+        <v>9</v>
+      </c>
+      <c r="K6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -872,8 +1042,14 @@
         <f t="shared" si="0"/>
         <v>444</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H7" t="s">
+        <v>129</v>
+      </c>
+      <c r="I7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -891,8 +1067,14 @@
         <f t="shared" si="0"/>
         <v>522</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H8" t="s">
+        <v>127</v>
+      </c>
+      <c r="I8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -910,8 +1092,14 @@
         <f t="shared" si="0"/>
         <v>549</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H9" t="s">
+        <v>127</v>
+      </c>
+      <c r="I9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -929,8 +1117,14 @@
         <f t="shared" si="0"/>
         <v>483</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H10" t="s">
+        <v>127</v>
+      </c>
+      <c r="I10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -948,8 +1142,14 @@
         <f t="shared" si="0"/>
         <v>567</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H11" t="s">
+        <v>130</v>
+      </c>
+      <c r="I11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -967,8 +1167,14 @@
         <f t="shared" si="0"/>
         <v>1182</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H12" t="s">
+        <v>130</v>
+      </c>
+      <c r="I12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -986,8 +1192,14 @@
         <f t="shared" si="0"/>
         <v>828</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H13" t="s">
+        <v>130</v>
+      </c>
+      <c r="I13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1005,8 +1217,14 @@
         <f t="shared" si="0"/>
         <v>558</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H14" t="s">
+        <v>161</v>
+      </c>
+      <c r="I14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1024,8 +1242,14 @@
         <f t="shared" si="0"/>
         <v>648</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H15" t="s">
+        <v>161</v>
+      </c>
+      <c r="I15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1042,6 +1266,12 @@
       <c r="E16">
         <f t="shared" si="0"/>
         <v>687</v>
+      </c>
+      <c r="H16" t="s">
+        <v>161</v>
+      </c>
+      <c r="I16">
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -2009,7 +2239,7 @@
         <v>231</v>
       </c>
       <c r="E67">
-        <f t="shared" ref="E67:E120" si="2">D67*3</f>
+        <f t="shared" ref="E67:E150" si="2">D67*3</f>
         <v>693</v>
       </c>
     </row>
@@ -2024,7 +2254,7 @@
         <v>127</v>
       </c>
       <c r="D68">
-        <f t="shared" ref="D68:D120" si="3">B68+C68</f>
+        <f t="shared" ref="D68:D150" si="3">B68+C68</f>
         <v>246</v>
       </c>
       <c r="E68">
@@ -3018,6 +3248,576 @@
       <c r="E120">
         <f t="shared" si="2"/>
         <v>513</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>131</v>
+      </c>
+      <c r="B121">
+        <v>170</v>
+      </c>
+      <c r="C121">
+        <v>158</v>
+      </c>
+      <c r="D121">
+        <f t="shared" si="3"/>
+        <v>328</v>
+      </c>
+      <c r="E121">
+        <f t="shared" si="2"/>
+        <v>984</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>132</v>
+      </c>
+      <c r="B122">
+        <v>59</v>
+      </c>
+      <c r="C122">
+        <v>68</v>
+      </c>
+      <c r="D122">
+        <f t="shared" si="3"/>
+        <v>127</v>
+      </c>
+      <c r="E122">
+        <f t="shared" si="2"/>
+        <v>381</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>133</v>
+      </c>
+      <c r="B123">
+        <v>116</v>
+      </c>
+      <c r="C123">
+        <v>154</v>
+      </c>
+      <c r="D123">
+        <f t="shared" si="3"/>
+        <v>270</v>
+      </c>
+      <c r="E123">
+        <f t="shared" si="2"/>
+        <v>810</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>134</v>
+      </c>
+      <c r="B124">
+        <v>184</v>
+      </c>
+      <c r="C124">
+        <v>151</v>
+      </c>
+      <c r="D124">
+        <f t="shared" si="3"/>
+        <v>335</v>
+      </c>
+      <c r="E124">
+        <f t="shared" si="2"/>
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>135</v>
+      </c>
+      <c r="B125">
+        <v>192</v>
+      </c>
+      <c r="C125">
+        <v>163</v>
+      </c>
+      <c r="D125">
+        <f t="shared" si="3"/>
+        <v>355</v>
+      </c>
+      <c r="E125">
+        <f t="shared" si="2"/>
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>136</v>
+      </c>
+      <c r="B126">
+        <v>191</v>
+      </c>
+      <c r="C126">
+        <v>155</v>
+      </c>
+      <c r="D126">
+        <f t="shared" si="3"/>
+        <v>346</v>
+      </c>
+      <c r="E126">
+        <f t="shared" si="2"/>
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>137</v>
+      </c>
+      <c r="B127">
+        <v>59</v>
+      </c>
+      <c r="C127">
+        <v>63</v>
+      </c>
+      <c r="D127">
+        <f t="shared" si="3"/>
+        <v>122</v>
+      </c>
+      <c r="E127">
+        <f t="shared" si="2"/>
+        <v>366</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>138</v>
+      </c>
+      <c r="B128">
+        <v>124</v>
+      </c>
+      <c r="C128">
+        <v>135</v>
+      </c>
+      <c r="D128">
+        <f t="shared" si="3"/>
+        <v>259</v>
+      </c>
+      <c r="E128">
+        <f t="shared" si="2"/>
+        <v>777</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>139</v>
+      </c>
+      <c r="B129">
+        <v>78</v>
+      </c>
+      <c r="C129">
+        <v>83</v>
+      </c>
+      <c r="D129">
+        <f t="shared" si="3"/>
+        <v>161</v>
+      </c>
+      <c r="E129">
+        <f t="shared" si="2"/>
+        <v>483</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>140</v>
+      </c>
+      <c r="B130">
+        <v>79</v>
+      </c>
+      <c r="C130">
+        <v>81</v>
+      </c>
+      <c r="D130">
+        <f t="shared" si="3"/>
+        <v>160</v>
+      </c>
+      <c r="E130">
+        <f t="shared" si="2"/>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>141</v>
+      </c>
+      <c r="B131">
+        <v>97</v>
+      </c>
+      <c r="C131">
+        <v>94</v>
+      </c>
+      <c r="D131">
+        <f t="shared" si="3"/>
+        <v>191</v>
+      </c>
+      <c r="E131">
+        <f t="shared" si="2"/>
+        <v>573</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>142</v>
+      </c>
+      <c r="B132">
+        <v>189</v>
+      </c>
+      <c r="C132">
+        <v>192</v>
+      </c>
+      <c r="D132">
+        <f t="shared" si="3"/>
+        <v>381</v>
+      </c>
+      <c r="E132">
+        <f t="shared" si="2"/>
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>143</v>
+      </c>
+      <c r="B133">
+        <v>189</v>
+      </c>
+      <c r="C133">
+        <v>217</v>
+      </c>
+      <c r="D133">
+        <f t="shared" si="3"/>
+        <v>406</v>
+      </c>
+      <c r="E133">
+        <f t="shared" si="2"/>
+        <v>1218</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>144</v>
+      </c>
+      <c r="B134">
+        <v>230</v>
+      </c>
+      <c r="C134">
+        <v>211</v>
+      </c>
+      <c r="D134">
+        <f t="shared" si="3"/>
+        <v>441</v>
+      </c>
+      <c r="E134">
+        <f t="shared" si="2"/>
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>145</v>
+      </c>
+      <c r="B135">
+        <v>68</v>
+      </c>
+      <c r="C135">
+        <v>71</v>
+      </c>
+      <c r="D135">
+        <f t="shared" si="3"/>
+        <v>139</v>
+      </c>
+      <c r="E135">
+        <f t="shared" si="2"/>
+        <v>417</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>146</v>
+      </c>
+      <c r="B136">
+        <v>120</v>
+      </c>
+      <c r="C136">
+        <v>115</v>
+      </c>
+      <c r="D136">
+        <f t="shared" si="3"/>
+        <v>235</v>
+      </c>
+      <c r="E136">
+        <f t="shared" si="2"/>
+        <v>705</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>147</v>
+      </c>
+      <c r="B137">
+        <v>69</v>
+      </c>
+      <c r="C137">
+        <v>58</v>
+      </c>
+      <c r="D137">
+        <f t="shared" si="3"/>
+        <v>127</v>
+      </c>
+      <c r="E137">
+        <f t="shared" si="2"/>
+        <v>381</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>148</v>
+      </c>
+      <c r="B138">
+        <v>100</v>
+      </c>
+      <c r="C138">
+        <v>101</v>
+      </c>
+      <c r="D138">
+        <f t="shared" si="3"/>
+        <v>201</v>
+      </c>
+      <c r="E138">
+        <f t="shared" si="2"/>
+        <v>603</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>149</v>
+      </c>
+      <c r="B139">
+        <v>100</v>
+      </c>
+      <c r="C139">
+        <v>102</v>
+      </c>
+      <c r="D139">
+        <f t="shared" si="3"/>
+        <v>202</v>
+      </c>
+      <c r="E139">
+        <f t="shared" si="2"/>
+        <v>606</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>150</v>
+      </c>
+      <c r="B140">
+        <v>120</v>
+      </c>
+      <c r="C140">
+        <v>120</v>
+      </c>
+      <c r="D140">
+        <f t="shared" si="3"/>
+        <v>240</v>
+      </c>
+      <c r="E140">
+        <f t="shared" si="2"/>
+        <v>720</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>151</v>
+      </c>
+      <c r="B141">
+        <v>142</v>
+      </c>
+      <c r="C141">
+        <v>165</v>
+      </c>
+      <c r="D141">
+        <f t="shared" si="3"/>
+        <v>307</v>
+      </c>
+      <c r="E141">
+        <f t="shared" si="2"/>
+        <v>921</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
+        <v>152</v>
+      </c>
+      <c r="B142">
+        <v>184</v>
+      </c>
+      <c r="C142">
+        <v>218</v>
+      </c>
+      <c r="D142">
+        <f t="shared" si="3"/>
+        <v>402</v>
+      </c>
+      <c r="E142">
+        <f t="shared" si="2"/>
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>153</v>
+      </c>
+      <c r="B143">
+        <v>157</v>
+      </c>
+      <c r="C143">
+        <v>141</v>
+      </c>
+      <c r="D143">
+        <f t="shared" si="3"/>
+        <v>298</v>
+      </c>
+      <c r="E143">
+        <f t="shared" si="2"/>
+        <v>894</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>154</v>
+      </c>
+      <c r="B144">
+        <v>170</v>
+      </c>
+      <c r="C144">
+        <v>143</v>
+      </c>
+      <c r="D144">
+        <f t="shared" si="3"/>
+        <v>313</v>
+      </c>
+      <c r="E144">
+        <f t="shared" si="2"/>
+        <v>939</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>155</v>
+      </c>
+      <c r="B145">
+        <v>193</v>
+      </c>
+      <c r="C145">
+        <v>218</v>
+      </c>
+      <c r="D145">
+        <f t="shared" si="3"/>
+        <v>411</v>
+      </c>
+      <c r="E145">
+        <f t="shared" si="2"/>
+        <v>1233</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>156</v>
+      </c>
+      <c r="B146">
+        <v>134</v>
+      </c>
+      <c r="C146">
+        <v>117</v>
+      </c>
+      <c r="D146">
+        <f t="shared" si="3"/>
+        <v>251</v>
+      </c>
+      <c r="E146">
+        <f t="shared" si="2"/>
+        <v>753</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>157</v>
+      </c>
+      <c r="B147">
+        <v>107</v>
+      </c>
+      <c r="C147">
+        <v>114</v>
+      </c>
+      <c r="D147">
+        <f t="shared" si="3"/>
+        <v>221</v>
+      </c>
+      <c r="E147">
+        <f t="shared" si="2"/>
+        <v>663</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
+        <v>158</v>
+      </c>
+      <c r="B148">
+        <v>36</v>
+      </c>
+      <c r="C148">
+        <v>36</v>
+      </c>
+      <c r="D148">
+        <f t="shared" si="3"/>
+        <v>72</v>
+      </c>
+      <c r="E148">
+        <f t="shared" si="2"/>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
+        <v>159</v>
+      </c>
+      <c r="B149">
+        <v>87</v>
+      </c>
+      <c r="C149">
+        <v>86</v>
+      </c>
+      <c r="D149">
+        <f t="shared" si="3"/>
+        <v>173</v>
+      </c>
+      <c r="E149">
+        <f t="shared" si="2"/>
+        <v>519</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
+        <v>160</v>
+      </c>
+      <c r="B150">
+        <v>119</v>
+      </c>
+      <c r="C150">
+        <v>122</v>
+      </c>
+      <c r="D150">
+        <f t="shared" si="3"/>
+        <v>241</v>
+      </c>
+      <c r="E150">
+        <f t="shared" si="2"/>
+        <v>723</v>
       </c>
     </row>
   </sheetData>

</xml_diff>